<commit_message>
Updated the page names for Subpopulation and LOT pages
</commit_message>
<xml_diff>
--- a/Testdata/ExcludedStudies_LiveSLR_Data.xlsx
+++ b/Testdata/ExcludedStudies_LiveSLR_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F19D6E2-EDED-47E7-9117-5CFADBA2E4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855C92D2-5D58-419A-9F16-88AB662C7682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -241,24 +241,12 @@
     <t>Name</t>
   </si>
   <si>
-    <t>lot_section1</t>
-  </si>
-  <si>
-    <t>lot_section1_checkbox</t>
-  </si>
-  <si>
     <t>intervention_section6</t>
   </si>
   <si>
     <t>intervention_section6_checkbox</t>
   </si>
   <si>
-    <t>sub_pop_section2</t>
-  </si>
-  <si>
-    <t>sub_pop_section2_checkbox</t>
-  </si>
-  <si>
     <t>intervention_section4</t>
   </si>
   <si>
@@ -292,9 +280,6 @@
     <t>sectionname</t>
   </si>
   <si>
-    <t>lot_section</t>
-  </si>
-  <si>
     <t>intervention_section</t>
   </si>
   <si>
@@ -304,9 +289,6 @@
     <t>reported_variable_section</t>
   </si>
   <si>
-    <t>sub_pop_section</t>
-  </si>
-  <si>
     <t>ExpectedSourceTemplateFile</t>
   </si>
   <si>
@@ -347,6 +329,24 @@
   </si>
   <si>
     <t>StandardExcelReport-NewImportLogic_1-Test_Automation_1-Real-world Evidence-2023_</t>
+  </si>
+  <si>
+    <t>pop_filter2_section1</t>
+  </si>
+  <si>
+    <t>pop_filter2_section1_checkbox</t>
+  </si>
+  <si>
+    <t>pop_filter2_section</t>
+  </si>
+  <si>
+    <t>pop_filter1_section2</t>
+  </si>
+  <si>
+    <t>pop_filter1_section2_checkbox</t>
+  </si>
+  <si>
+    <t>pop_filter1_section</t>
   </si>
 </sst>
 </file>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,19 +714,19 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" t="s">
         <v>84</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J1" t="s">
-        <v>90</v>
       </c>
       <c r="K1" t="s">
         <v>4</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
         <v>60</v>
@@ -755,22 +755,22 @@
         <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="I2" s="2">
         <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="K2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L2" t="s">
         <v>11</v>
@@ -781,22 +781,22 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I3" s="2">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="L3" t="s">
         <v>17</v>
@@ -807,7 +807,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -816,13 +816,13 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I4" s="2">
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="L4" t="s">
         <v>19</v>
@@ -833,7 +833,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -842,13 +842,13 @@
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I5" s="2">
         <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="L5" t="s">
         <v>21</v>
@@ -859,13 +859,13 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I6" s="2">
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="L6" t="s">
         <v>23</v>
@@ -876,7 +876,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I7" s="2">
         <v>2</v>
@@ -887,23 +887,23 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I8" s="2">
         <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
         <v>60</v>
@@ -918,19 +918,19 @@
         <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="I10">
         <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="K10" t="s">
         <v>63</v>
@@ -944,22 +944,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="H11" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="K11" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L11" t="s">
         <v>27</v>
@@ -970,22 +970,22 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I12">
         <v>6</v>
       </c>
       <c r="K12" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="L12" t="s">
         <v>29</v>
@@ -996,7 +996,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
@@ -1005,7 +1005,7 @@
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I14">
         <v>2</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I16">
         <v>3</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
         <v>60</v>
@@ -1064,19 +1064,19 @@
         <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="H18" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="I18">
         <v>24</v>
       </c>
       <c r="J18" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="L18" t="s">
         <v>34</v>
@@ -1084,16 +1084,16 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="G19" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="H19" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="I19">
         <v>12</v>
@@ -1104,16 +1104,16 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H20" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I20">
         <v>3</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
@@ -1133,7 +1133,7 @@
         <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I21">
         <v>4</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I22">
         <v>2</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I24">
         <v>3</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
         <v>60</v>
@@ -1186,19 +1186,19 @@
         <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="H26" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="I26">
         <v>102</v>
       </c>
       <c r="J26" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="L26" t="s">
         <v>39</v>
@@ -1206,16 +1206,16 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" t="s">
         <v>81</v>
-      </c>
-      <c r="F27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G27" t="s">
-        <v>94</v>
-      </c>
-      <c r="H27" t="s">
-        <v>86</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F28" t="s">
         <v>9</v>
@@ -1235,7 +1235,7 @@
         <v>10</v>
       </c>
       <c r="H28" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I28">
         <v>18</v>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
@@ -1255,7 +1255,7 @@
         <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I29">
         <v>33</v>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I30">
         <v>37</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I31">
         <v>2</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I32">
         <v>13</v>

</xml_diff>